<commit_message>
self assessment from the sprint A.
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Desktop\ISEP\LAPR2\Project2\lei-24-s2-1dh-g084\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E6F695-B244-46C0-BA58-90C835288F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D1CC02-EA7F-4199-A4D7-B7BD8847F8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="134">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -66,51 +66,6 @@
   </si>
   <si>
     <t>List A</t>
-  </si>
-  <si>
-    <t>Student 1</t>
-  </si>
-  <si>
-    <t>Student 2</t>
-  </si>
-  <si>
-    <t>Student 3</t>
-  </si>
-  <si>
-    <t>Student 4</t>
-  </si>
-  <si>
-    <t>Student 5</t>
-  </si>
-  <si>
-    <t>Student 6</t>
-  </si>
-  <si>
-    <t>Student 7</t>
-  </si>
-  <si>
-    <t>Student 8</t>
-  </si>
-  <si>
-    <t>Student 9</t>
-  </si>
-  <si>
-    <t>Student 10</t>
-  </si>
-  <si>
-    <t>Student 11</t>
-  </si>
-  <si>
-    <t>Student 12</t>
-  </si>
-  <si>
-    <t>Student 13</t>
-  </si>
-  <si>
-    <t>Student 14</t>
-  </si>
-  <si>
-    <t>Student 15</t>
   </si>
   <si>
     <t>Instructions:</t>
@@ -512,6 +467,24 @@
   </si>
   <si>
     <t>LAPR3 Project Group and Self-assessment v4.0</t>
+  </si>
+  <si>
+    <t>Joana Gama</t>
+  </si>
+  <si>
+    <t>Bruno Teixeira</t>
+  </si>
+  <si>
+    <t>Francisco Pinho</t>
+  </si>
+  <si>
+    <t>Ricardo Meireles</t>
+  </si>
+  <si>
+    <t>Samuel Leite</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -1779,8 +1752,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1793,7 +1766,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1853,74 +1826,74 @@
       <c r="C9" s="1"/>
       <c r="D9" s="42" t="str">
         <f>C10</f>
-        <v>Student 1</v>
+        <v>Joana Gama</v>
       </c>
       <c r="E9" s="43" t="str">
         <f>C11</f>
-        <v>Student 2</v>
+        <v>Bruno Teixeira</v>
       </c>
       <c r="F9" s="43" t="str">
         <f>C12</f>
-        <v>Student 3</v>
+        <v>Francisco Pinho</v>
       </c>
       <c r="G9" s="43" t="str">
         <f>C13</f>
-        <v>Student 4</v>
+        <v>Ricardo Meireles</v>
       </c>
       <c r="H9" s="43" t="str">
         <f>C14</f>
-        <v>Student 5</v>
+        <v>Samuel Leite</v>
       </c>
       <c r="I9" s="43" t="str">
         <f>C15</f>
-        <v>Student 6</v>
+        <v>Null</v>
       </c>
       <c r="J9" s="43" t="str">
         <f>C16</f>
-        <v>Student 7</v>
+        <v>Null</v>
       </c>
       <c r="K9" s="43" t="str">
         <f>C17</f>
-        <v>Student 8</v>
+        <v>Null</v>
       </c>
       <c r="L9" s="43" t="str">
         <f>C18</f>
-        <v>Student 9</v>
+        <v>Null</v>
       </c>
       <c r="M9" s="43" t="str">
         <f>C19</f>
-        <v>Student 10</v>
+        <v>Null</v>
       </c>
       <c r="N9" s="43" t="str">
         <f>C20</f>
-        <v>Student 11</v>
+        <v>Null</v>
       </c>
       <c r="O9" s="43" t="str">
         <f>C21</f>
-        <v>Student 12</v>
+        <v>Null</v>
       </c>
       <c r="P9" s="43" t="str">
         <f>C22</f>
-        <v>Student 13</v>
+        <v>Null</v>
       </c>
       <c r="Q9" s="43" t="str">
         <f>C23</f>
-        <v>Student 14</v>
+        <v>Null</v>
       </c>
       <c r="R9" s="43" t="str">
         <f>C24</f>
-        <v>Student 15</v>
+        <v>Null</v>
       </c>
       <c r="S9" s="44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="38"/>
@@ -1942,10 +1915,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="63"/>
       <c r="C11" s="8" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="36"/>
@@ -1967,10 +1940,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="63"/>
       <c r="C12" s="8" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
@@ -1992,10 +1965,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="63"/>
       <c r="C13" s="8" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -2017,10 +1990,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="63"/>
       <c r="C14" s="8" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2045,7 +2018,7 @@
     <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="63"/>
       <c r="C15" s="8" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2070,7 +2043,7 @@
     <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="63"/>
       <c r="C16" s="8" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2095,7 +2068,7 @@
     <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="63"/>
       <c r="C17" s="8" t="s">
-        <v>14</v>
+        <v>133</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2120,7 +2093,7 @@
     <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="63"/>
       <c r="C18" s="8" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2145,7 +2118,7 @@
     <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2170,7 +2143,7 @@
     <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="63"/>
       <c r="C20" s="8" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2195,7 +2168,7 @@
     <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="63"/>
       <c r="C21" s="8" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2220,7 +2193,7 @@
     <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="63"/>
       <c r="C22" s="8" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2245,7 +2218,7 @@
     <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="63"/>
       <c r="C23" s="8" t="s">
-        <v>20</v>
+        <v>133</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2269,8 +2242,8 @@
     </row>
     <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="64"/>
-      <c r="C24" s="40" t="s">
-        <v>21</v>
+      <c r="C24" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -2361,22 +2334,22 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2384,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2392,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2400,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2408,7 +2381,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2416,7 +2389,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2424,7 +2397,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2461,22 +2434,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="30" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2503,22 +2476,22 @@
       <c r="C4" s="71"/>
       <c r="D4" s="69"/>
       <c r="E4" s="14" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2527,22 +2500,22 @@
       <c r="C5" s="71"/>
       <c r="D5" s="69"/>
       <c r="E5" s="22" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2551,22 +2524,22 @@
       <c r="C6" s="29"/>
       <c r="D6" s="60"/>
       <c r="E6" s="31" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2575,22 +2548,22 @@
       <c r="C7" s="29"/>
       <c r="D7" s="60"/>
       <c r="E7" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J7" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2599,22 +2572,22 @@
       <c r="C8" s="29"/>
       <c r="D8" s="60"/>
       <c r="E8" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2623,22 +2596,22 @@
       <c r="C9" s="29"/>
       <c r="D9" s="60"/>
       <c r="E9" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2647,22 +2620,22 @@
       <c r="C10" s="29"/>
       <c r="D10" s="60"/>
       <c r="E10" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2671,22 +2644,22 @@
       <c r="C11" s="29"/>
       <c r="D11" s="60"/>
       <c r="E11" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J11" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2695,22 +2668,22 @@
       <c r="C12" s="29"/>
       <c r="D12" s="60"/>
       <c r="E12" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J12" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2719,22 +2692,22 @@
       <c r="C13" s="29"/>
       <c r="D13" s="60"/>
       <c r="E13" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2743,22 +2716,22 @@
       <c r="C14" s="29"/>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2767,22 +2740,22 @@
       <c r="C15" s="29"/>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2791,22 +2764,22 @@
       <c r="C16" s="29"/>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2815,22 +2788,22 @@
       <c r="C17" s="29"/>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2839,22 +2812,22 @@
       <c r="C18" s="29"/>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2863,22 +2836,22 @@
       <c r="C19" s="29"/>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2887,22 +2860,22 @@
       <c r="C20" s="29"/>
       <c r="D20" s="60"/>
       <c r="E20" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2911,22 +2884,22 @@
       <c r="C21" s="29"/>
       <c r="D21" s="60"/>
       <c r="E21" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2935,22 +2908,22 @@
       <c r="C22" s="29"/>
       <c r="D22" s="60"/>
       <c r="E22" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2959,22 +2932,22 @@
       <c r="C23" s="29"/>
       <c r="D23" s="60"/>
       <c r="E23" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2983,22 +2956,22 @@
       <c r="C24" s="29"/>
       <c r="D24" s="60"/>
       <c r="E24" s="14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3007,22 +2980,22 @@
       <c r="C25" s="54"/>
       <c r="D25" s="61"/>
       <c r="E25" s="22" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="J25" s="33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3089,7 +3062,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3109,70 +3082,70 @@
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C3" s="20" t="str">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Student 1</v>
+        <v>Joana Gama</v>
       </c>
       <c r="D3" s="20" t="str">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Student 2</v>
+        <v>Bruno Teixeira</v>
       </c>
       <c r="E3" s="20" t="str">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Student 3</v>
+        <v>Francisco Pinho</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Student 4</v>
+        <v>Ricardo Meireles</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Student 5</v>
+        <v>Samuel Leite</v>
       </c>
       <c r="H3" s="20" t="str">
         <f>'Group and Self Assessment'!C15</f>
-        <v>Student 6</v>
+        <v>Null</v>
       </c>
       <c r="I3" s="20" t="str">
         <f>'Group and Self Assessment'!C16</f>
-        <v>Student 7</v>
+        <v>Null</v>
       </c>
       <c r="J3" s="20" t="str">
         <f>'Group and Self Assessment'!C17</f>
-        <v>Student 8</v>
+        <v>Null</v>
       </c>
       <c r="K3" s="20" t="str">
         <f>'Group and Self Assessment'!C18</f>
-        <v>Student 9</v>
+        <v>Null</v>
       </c>
       <c r="L3" s="20" t="str">
         <f>'Group and Self Assessment'!C19</f>
-        <v>Student 10</v>
+        <v>Null</v>
       </c>
       <c r="M3" s="20" t="str">
         <f>'Group and Self Assessment'!C20</f>
-        <v>Student 11</v>
+        <v>Null</v>
       </c>
       <c r="N3" s="20" t="str">
         <f>'Group and Self Assessment'!C21</f>
-        <v>Student 12</v>
+        <v>Null</v>
       </c>
       <c r="O3" s="20" t="str">
         <f>'Group and Self Assessment'!C22</f>
-        <v>Student 13</v>
+        <v>Null</v>
       </c>
       <c r="P3" s="20" t="str">
         <f>'Group and Self Assessment'!C23</f>
-        <v>Student 14</v>
+        <v>Null</v>
       </c>
       <c r="Q3" s="20" t="str">
         <f>'Group and Self Assessment'!C24</f>
-        <v>Student 15</v>
+        <v>Null</v>
       </c>
       <c r="R3" s="20" t="s">
         <v>5</v>
@@ -3202,15 +3175,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3235,29 +3208,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B5" s="17">
         <v>0.2</v>
@@ -3282,29 +3255,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B6" s="17">
         <v>0.5</v>
@@ -3329,29 +3302,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
@@ -3376,29 +3349,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
@@ -3476,7 +3449,7 @@
     </row>
     <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
@@ -3568,7 +3541,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -3589,7 +3562,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="13"/>
@@ -3608,70 +3581,70 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C3" s="20" t="str">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Student 1</v>
+        <v>Joana Gama</v>
       </c>
       <c r="D3" s="20" t="str">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Student 2</v>
+        <v>Bruno Teixeira</v>
       </c>
       <c r="E3" s="20" t="str">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Student 3</v>
+        <v>Francisco Pinho</v>
       </c>
       <c r="F3" s="20" t="str">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Student 4</v>
+        <v>Ricardo Meireles</v>
       </c>
       <c r="G3" s="20" t="str">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Student 5</v>
+        <v>Samuel Leite</v>
       </c>
       <c r="H3" s="20" t="str">
         <f>'Group and Self Assessment'!C15</f>
-        <v>Student 6</v>
+        <v>Null</v>
       </c>
       <c r="I3" s="20" t="str">
         <f>'Group and Self Assessment'!C16</f>
-        <v>Student 7</v>
+        <v>Null</v>
       </c>
       <c r="J3" s="20" t="str">
         <f>'Group and Self Assessment'!C17</f>
-        <v>Student 8</v>
+        <v>Null</v>
       </c>
       <c r="K3" s="20" t="str">
         <f>'Group and Self Assessment'!C18</f>
-        <v>Student 9</v>
+        <v>Null</v>
       </c>
       <c r="L3" s="20" t="str">
         <f>'Group and Self Assessment'!C19</f>
-        <v>Student 10</v>
+        <v>Null</v>
       </c>
       <c r="M3" s="20" t="str">
         <f>'Group and Self Assessment'!C20</f>
-        <v>Student 11</v>
+        <v>Null</v>
       </c>
       <c r="N3" s="20" t="str">
         <f>'Group and Self Assessment'!C21</f>
-        <v>Student 12</v>
+        <v>Null</v>
       </c>
       <c r="O3" s="20" t="str">
         <f>'Group and Self Assessment'!C22</f>
-        <v>Student 13</v>
+        <v>Null</v>
       </c>
       <c r="P3" s="20" t="str">
         <f>'Group and Self Assessment'!C23</f>
-        <v>Student 14</v>
+        <v>Null</v>
       </c>
       <c r="Q3" s="20" t="str">
         <f>'Group and Self Assessment'!C24</f>
-        <v>Student 15</v>
+        <v>Null</v>
       </c>
       <c r="R3" s="20" t="s">
         <v>5</v>
@@ -3701,15 +3674,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3734,29 +3707,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S4" s="59" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="T4" s="59" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="W4" s="59" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="X4" s="59" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
@@ -3781,29 +3754,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S5" s="59" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="T5" s="59" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="U5" s="59" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="V5" s="59" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="W5" s="59" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="X5" s="59" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B6" s="17">
         <v>0.05</v>
@@ -3828,29 +3801,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="T6" s="59" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="U6" s="59" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="V6" s="59" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="W6" s="59" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="X6" s="59" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B7" s="17">
         <v>0.05</v>
@@ -3875,29 +3848,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="T7" s="59" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="V7" s="59" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="W7" s="59" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="X7" s="59" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B8" s="17">
         <v>0.1</v>
@@ -3922,29 +3895,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S8" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="U8" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="V8" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="T8" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="U8" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="V8" s="59" t="s">
-        <v>113</v>
-      </c>
       <c r="W8" s="59" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="X8" s="59" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B9" s="17">
         <v>0.05</v>
@@ -3969,25 +3942,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S9" s="59" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="T9" s="59" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="U9" s="59"/>
       <c r="V9" s="59" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="W9" s="59"/>
       <c r="X9" s="59" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B10" s="17">
         <v>0.1</v>
@@ -4012,29 +3985,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S10" s="59" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="T10" s="59" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="U10" s="59" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="V10" s="59" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="W10" s="59" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="X10" s="59" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
@@ -4059,29 +4032,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="T11" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="U11" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="V11" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="W11" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="X11" s="59" t="s">
         <v>117</v>
-      </c>
-      <c r="T11" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="U11" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V11" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W11" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X11" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
@@ -4106,29 +4079,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="T12" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="V12" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="W12" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="X12" s="59" t="s">
         <v>117</v>
-      </c>
-      <c r="T12" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="U12" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V12" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W12" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X12" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
     <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
@@ -4153,29 +4126,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="59" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="T13" s="59" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="U13" s="59" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="W13" s="59" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="X13" s="59" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
     <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
@@ -4200,29 +4173,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="T14" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="V14" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="W14" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="X14" s="59" t="s">
         <v>117</v>
-      </c>
-      <c r="T14" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="U14" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="V14" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="W14" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="X14" s="59" t="s">
-        <v>132</v>
       </c>
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B15" s="18">
         <f>SUM(B4:B14)</f>
@@ -4300,7 +4273,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
@@ -4388,6 +4361,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4571,15 +4553,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4587,6 +4560,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4604,25 +4585,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Self assessment from the sprint A - final version.
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Desktop\ISEP\LAPR2\Project2\lei-24-s2-1dh-g084\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1230744_isep_ipp_pt/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D1CC02-EA7F-4199-A4D7-B7BD8847F8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{8C2E7610-F121-4699-979F-0943CFF4594F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBE6AE67-F902-4714-BD2C-97894CC37270}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="ItemEval">[1]!Table2[ItemEval]</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="129">
+  <si>
+    <t>LAPR3 Project Group and Self-assessment v4.0</t>
+  </si>
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -66,6 +69,9 @@
   </si>
   <si>
     <t>List A</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
   <si>
     <t>Instructions:</t>
@@ -164,16 +170,13 @@
     <t>The students  have exceeded expectations </t>
   </si>
   <si>
+    <t>Project Development Self-Assessment</t>
+  </si>
+  <si>
+    <t>Rubric</t>
+  </si>
+  <si>
     <t>Weight</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Project Development Self-Assessment</t>
-  </si>
-  <si>
-    <t>Rubric</t>
   </si>
   <si>
     <t>Teacher
@@ -283,6 +286,9 @@
 data</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Total (0-20)</t>
   </si>
   <si>
@@ -464,27 +470,6 @@
   </si>
   <si>
     <t>Overall Sprint management</t>
-  </si>
-  <si>
-    <t>LAPR3 Project Group and Self-assessment v4.0</t>
-  </si>
-  <si>
-    <t>Joana Gama</t>
-  </si>
-  <si>
-    <t>Bruno Teixeira</t>
-  </si>
-  <si>
-    <t>Francisco Pinho</t>
-  </si>
-  <si>
-    <t>Ricardo Meireles</t>
-  </si>
-  <si>
-    <t>Samuel Leite</t>
-  </si>
-  <si>
-    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -1452,10 +1437,14 @@
 </inkml:ink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1493,7 +1482,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1599,7 +1588,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1741,7 +1730,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1752,8 +1741,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1766,14 +1755,14 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1784,18 +1773,18 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1803,7 +1792,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="66"/>
       <c r="G8" s="66"/>
@@ -1824,25 +1813,25 @@
     <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="42" t="str">
+      <c r="D9" s="42">
         <f>C10</f>
-        <v>Joana Gama</v>
-      </c>
-      <c r="E9" s="43" t="str">
+        <v>1230399</v>
+      </c>
+      <c r="E9" s="43">
         <f>C11</f>
-        <v>Bruno Teixeira</v>
-      </c>
-      <c r="F9" s="43" t="str">
+        <v>1230741</v>
+      </c>
+      <c r="F9" s="43">
         <f>C12</f>
-        <v>Francisco Pinho</v>
-      </c>
-      <c r="G9" s="43" t="str">
+        <v>1231235</v>
+      </c>
+      <c r="G9" s="43">
         <f>C13</f>
-        <v>Ricardo Meireles</v>
-      </c>
-      <c r="H9" s="43" t="str">
+        <v>1230744</v>
+      </c>
+      <c r="H9" s="43">
         <f>C14</f>
-        <v>Samuel Leite</v>
+        <v>1191647</v>
       </c>
       <c r="I9" s="43" t="str">
         <f>C15</f>
@@ -1885,21 +1874,31 @@
         <v>Null</v>
       </c>
       <c r="S9" s="44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="37">
+        <v>1230399</v>
+      </c>
+      <c r="D10" s="36">
+        <v>4</v>
+      </c>
+      <c r="E10" s="38">
+        <v>4</v>
+      </c>
+      <c r="F10" s="39">
+        <v>3</v>
+      </c>
+      <c r="G10" s="39">
+        <v>4</v>
+      </c>
+      <c r="H10" s="39">
+        <v>3</v>
+      </c>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
@@ -1910,21 +1909,31 @@
       <c r="P10" s="39"/>
       <c r="Q10" s="39"/>
       <c r="R10" s="37"/>
-      <c r="S10" s="50" t="e">
+      <c r="S10" s="50">
         <f>AVERAGE(D10:R10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="63"/>
-      <c r="C11" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="C11" s="8">
+        <v>1230741</v>
+      </c>
+      <c r="D11" s="9">
+        <v>4</v>
+      </c>
+      <c r="E11" s="36">
+        <v>4</v>
+      </c>
+      <c r="F11" s="35">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8">
+        <v>4</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1935,21 +1944,31 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="10"/>
-      <c r="S11" s="51" t="e">
+      <c r="S11" s="51">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="63"/>
-      <c r="C12" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="8"/>
+      <c r="C12" s="8">
+        <v>1231235</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36">
+        <v>3</v>
+      </c>
+      <c r="G12" s="35">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3</v>
+      </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1960,21 +1979,31 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="51" t="e">
+      <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="63"/>
-      <c r="C13" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="35"/>
+      <c r="C13" s="8">
+        <v>1230744</v>
+      </c>
+      <c r="D13" s="8">
+        <v>4</v>
+      </c>
+      <c r="E13" s="8">
+        <v>4</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
+      <c r="G13" s="36">
+        <v>4</v>
+      </c>
+      <c r="H13" s="35">
+        <v>3</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1985,21 +2014,31 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="51" t="e">
+      <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="63"/>
-      <c r="C14" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="36"/>
+      <c r="C14" s="8">
+        <v>1191647</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8">
+        <v>4</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+      <c r="G14" s="9">
+        <v>4</v>
+      </c>
+      <c r="H14" s="36">
+        <v>3</v>
+      </c>
       <c r="I14" s="35"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -2010,15 +2049,15 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="10"/>
-      <c r="S14" s="51" t="e">
+      <c r="S14" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="63"/>
       <c r="C15" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2043,7 +2082,7 @@
     <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="63"/>
       <c r="C16" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2068,7 +2107,7 @@
     <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="63"/>
       <c r="C17" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2093,7 +2132,7 @@
     <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="63"/>
       <c r="C18" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2118,7 +2157,7 @@
     <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2143,7 +2182,7 @@
     <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="63"/>
       <c r="C20" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2168,7 +2207,7 @@
     <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="63"/>
       <c r="C21" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2193,7 +2232,7 @@
     <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="63"/>
       <c r="C22" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2218,7 +2257,7 @@
     <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="63"/>
       <c r="C23" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2243,7 +2282,7 @@
     <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="64"/>
       <c r="C24" s="8" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -2268,27 +2307,27 @@
     <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="46" t="e">
+        <v>6</v>
+      </c>
+      <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="46" t="e">
+        <v>4</v>
+      </c>
+      <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="46" t="e">
+        <v>4</v>
+      </c>
+      <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="46" t="e">
+        <v>3</v>
+      </c>
+      <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="46" t="e">
+        <v>4</v>
+      </c>
+      <c r="H25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="I25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -2334,22 +2373,22 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2357,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2365,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -2373,7 +2412,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -2381,7 +2420,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -2389,7 +2428,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -2397,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2420,8 +2459,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2434,22 +2473,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="30" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="62" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2476,22 +2515,22 @@
       <c r="C4" s="71"/>
       <c r="D4" s="69"/>
       <c r="E4" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2500,214 +2539,278 @@
       <c r="C5" s="71"/>
       <c r="D5" s="69"/>
       <c r="E5" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G5" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>1</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1231235</v>
+      </c>
+      <c r="C6" s="29">
+        <v>3</v>
+      </c>
+      <c r="D6" s="60">
+        <v>4</v>
+      </c>
+      <c r="E6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="F6" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="G6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="H6" s="32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="32" t="s">
+      <c r="I6" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>2</v>
+      </c>
+      <c r="B7" s="29">
+        <v>1230399</v>
+      </c>
+      <c r="C7" s="29">
+        <v>3</v>
+      </c>
+      <c r="D7" s="60">
+        <v>4</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="F7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="H7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="J7" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>3</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1230399</v>
+      </c>
+      <c r="C8" s="29">
+        <v>3</v>
+      </c>
+      <c r="D8" s="60">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="H8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="J8" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>4</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1230744</v>
+      </c>
+      <c r="C9" s="29">
+        <v>3</v>
+      </c>
+      <c r="D9" s="60">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="H9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="J9" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>5</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1230741</v>
+      </c>
+      <c r="C10" s="29">
+        <v>3</v>
+      </c>
+      <c r="D10" s="60">
+        <v>3</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="H10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="J10" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>6</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1231235</v>
+      </c>
+      <c r="C11" s="29">
+        <v>3</v>
+      </c>
+      <c r="D11" s="60">
+        <v>3</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="H11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="J11" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>7</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1191647</v>
+      </c>
+      <c r="C12" s="29">
+        <v>3</v>
+      </c>
+      <c r="D12" s="60">
+        <v>3</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="H12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="J12" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>8</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1230744</v>
+      </c>
+      <c r="C13" s="29">
+        <v>3</v>
+      </c>
+      <c r="D13" s="60">
+        <v>3</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="H13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="J13" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2716,22 +2819,22 @@
       <c r="C14" s="29"/>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2740,22 +2843,22 @@
       <c r="C15" s="29"/>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2764,22 +2867,22 @@
       <c r="C16" s="29"/>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2788,22 +2891,22 @@
       <c r="C17" s="29"/>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2812,22 +2915,22 @@
       <c r="C18" s="29"/>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2836,22 +2939,22 @@
       <c r="C19" s="29"/>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2860,22 +2963,22 @@
       <c r="C20" s="29"/>
       <c r="D20" s="60"/>
       <c r="E20" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2884,22 +2987,22 @@
       <c r="C21" s="29"/>
       <c r="D21" s="60"/>
       <c r="E21" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2908,22 +3011,22 @@
       <c r="C22" s="29"/>
       <c r="D22" s="60"/>
       <c r="E22" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2932,22 +3035,22 @@
       <c r="C23" s="29"/>
       <c r="D23" s="60"/>
       <c r="E23" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
@@ -2956,22 +3059,22 @@
       <c r="C24" s="29"/>
       <c r="D24" s="60"/>
       <c r="E24" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -2980,22 +3083,22 @@
       <c r="C25" s="54"/>
       <c r="D25" s="61"/>
       <c r="E25" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J25" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3039,8 +3142,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3080,32 +3183,32 @@
       <c r="O1" s="13"/>
     </row>
     <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="49.2" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="20" t="str">
+        <v>39</v>
+      </c>
+      <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Joana Gama</v>
-      </c>
-      <c r="D3" s="20" t="str">
+        <v>1230399</v>
+      </c>
+      <c r="D3" s="20">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Bruno Teixeira</v>
-      </c>
-      <c r="E3" s="20" t="str">
+        <v>1230741</v>
+      </c>
+      <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Francisco Pinho</v>
-      </c>
-      <c r="F3" s="20" t="str">
+        <v>1231235</v>
+      </c>
+      <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Ricardo Meireles</v>
-      </c>
-      <c r="G3" s="20" t="str">
+        <v>1230744</v>
+      </c>
+      <c r="G3" s="20">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Samuel Leite</v>
+        <v>1191647</v>
       </c>
       <c r="H3" s="20" t="str">
         <f>'Group and Self Assessment'!C15</f>
@@ -3148,7 +3251,7 @@
         <v>Null</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="26">
         <f>0</f>
@@ -3175,24 +3278,34 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="25">
+        <v>4</v>
+      </c>
+      <c r="D4" s="25">
+        <v>4</v>
+      </c>
+      <c r="E4" s="25">
+        <v>4</v>
+      </c>
+      <c r="F4" s="25">
+        <v>5</v>
+      </c>
+      <c r="G4" s="25">
+        <v>4</v>
+      </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -3203,43 +3316,53 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="27" t="e">
+      <c r="R4" s="27">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>#DIV/0!</v>
+        <v>4.2</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" s="17">
         <v>0.2</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="C5" s="25">
+        <v>4</v>
+      </c>
+      <c r="D5" s="25">
+        <v>4</v>
+      </c>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
+      <c r="F5" s="25">
+        <v>4</v>
+      </c>
+      <c r="G5" s="25">
+        <v>4</v>
+      </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
@@ -3250,43 +3373,53 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="27" t="e">
+      <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" s="17">
         <v>0.5</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="25">
+        <v>3</v>
+      </c>
+      <c r="D6" s="25">
+        <v>3</v>
+      </c>
+      <c r="E6" s="25">
+        <v>3</v>
+      </c>
+      <c r="F6" s="25">
+        <v>4</v>
+      </c>
+      <c r="G6" s="25">
+        <v>4</v>
+      </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -3297,34 +3430,34 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="27" t="e">
+      <c r="R6" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.4</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
@@ -3349,29 +3482,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
@@ -3379,23 +3512,23 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="1"/>
@@ -3449,28 +3582,28 @@
     </row>
     <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="H9" s="23">
         <f t="shared" si="2"/>
@@ -3541,8 +3674,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3562,7 +3695,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="13"/>
@@ -3579,32 +3712,32 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="49.8" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="20" t="str">
+        <v>39</v>
+      </c>
+      <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
-        <v>Joana Gama</v>
-      </c>
-      <c r="D3" s="20" t="str">
+        <v>1230399</v>
+      </c>
+      <c r="D3" s="20">
         <f>'Group and Self Assessment'!C11</f>
-        <v>Bruno Teixeira</v>
-      </c>
-      <c r="E3" s="20" t="str">
+        <v>1230741</v>
+      </c>
+      <c r="E3" s="20">
         <f>'Group and Self Assessment'!C12</f>
-        <v>Francisco Pinho</v>
-      </c>
-      <c r="F3" s="20" t="str">
+        <v>1231235</v>
+      </c>
+      <c r="F3" s="20">
         <f>'Group and Self Assessment'!C13</f>
-        <v>Ricardo Meireles</v>
-      </c>
-      <c r="G3" s="20" t="str">
+        <v>1230744</v>
+      </c>
+      <c r="G3" s="20">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Samuel Leite</v>
+        <v>1191647</v>
       </c>
       <c r="H3" s="20" t="str">
         <f>'Group and Self Assessment'!C15</f>
@@ -3647,7 +3780,7 @@
         <v>Null</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S3" s="57">
         <f>0</f>
@@ -3674,24 +3807,34 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="25">
+        <v>4</v>
+      </c>
+      <c r="D4" s="25">
+        <v>4</v>
+      </c>
+      <c r="E4" s="25">
+        <v>4</v>
+      </c>
+      <c r="F4" s="25">
+        <v>4</v>
+      </c>
+      <c r="G4" s="25">
+        <v>4</v>
+      </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -3702,43 +3845,53 @@
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="55" t="e">
+      <c r="R4" s="55">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S4" s="59" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T4" s="59" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="V4" s="59" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="W4" s="59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="X4" s="59" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="C5" s="25">
+        <v>4</v>
+      </c>
+      <c r="D5" s="25">
+        <v>4</v>
+      </c>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
+      <c r="F5" s="25">
+        <v>4</v>
+      </c>
+      <c r="G5" s="25">
+        <v>4</v>
+      </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
@@ -3749,43 +3902,53 @@
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="55" t="e">
+      <c r="R5" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
       <c r="S5" s="59" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="T5" s="59" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="U5" s="59" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="V5" s="59" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="W5" s="59" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="X5" s="59" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" s="17">
         <v>0.05</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="25">
+        <v>3</v>
+      </c>
+      <c r="D6" s="25">
+        <v>3</v>
+      </c>
+      <c r="E6" s="25">
+        <v>3</v>
+      </c>
+      <c r="F6" s="25">
+        <v>4</v>
+      </c>
+      <c r="G6" s="25">
+        <v>3</v>
+      </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -3796,43 +3959,53 @@
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="55" t="e">
+      <c r="R6" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.2</v>
       </c>
       <c r="S6" s="59" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T6" s="59" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U6" s="59" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="V6" s="59" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="W6" s="59" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="X6" s="59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B7" s="17">
         <v>0.05</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="25">
+        <v>4</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4</v>
+      </c>
+      <c r="F7" s="25">
+        <v>4</v>
+      </c>
+      <c r="G7" s="25">
+        <v>3</v>
+      </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
@@ -3843,43 +4016,53 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="55" t="e">
+      <c r="R7" s="55">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.8</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T7" s="59" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="V7" s="59" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="W7" s="59" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="X7" s="59" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B8" s="17">
         <v>0.1</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="C8" s="25">
+        <v>4</v>
+      </c>
+      <c r="D8" s="25">
+        <v>4</v>
+      </c>
+      <c r="E8" s="25">
+        <v>3</v>
+      </c>
+      <c r="F8" s="25">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25">
+        <v>3</v>
+      </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
@@ -3890,43 +4073,53 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
       <c r="Q8" s="25"/>
-      <c r="R8" s="55" t="e">
+      <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>#DIV/0!</v>
+        <v>3.6</v>
       </c>
       <c r="S8" s="59" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T8" s="59" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U8" s="59" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="V8" s="59" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="W8" s="59" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="X8" s="59" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B9" s="17">
         <v>0.05</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="C9" s="25">
+        <v>3</v>
+      </c>
+      <c r="D9" s="25">
+        <v>3</v>
+      </c>
+      <c r="E9" s="25">
+        <v>3</v>
+      </c>
+      <c r="F9" s="25">
+        <v>3</v>
+      </c>
+      <c r="G9" s="25">
+        <v>3</v>
+      </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
@@ -3937,39 +4130,49 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="25"/>
-      <c r="R9" s="55" t="e">
+      <c r="R9" s="55">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="S9" s="59" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T9" s="59" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="U9" s="59"/>
       <c r="V9" s="59" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="W9" s="59"/>
       <c r="X9" s="59" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B10" s="17">
         <v>0.1</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="C10" s="25">
+        <v>3</v>
+      </c>
+      <c r="D10" s="25">
+        <v>3</v>
+      </c>
+      <c r="E10" s="25">
+        <v>3</v>
+      </c>
+      <c r="F10" s="25">
+        <v>3</v>
+      </c>
+      <c r="G10" s="25">
+        <v>3</v>
+      </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
@@ -3980,34 +4183,34 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
       <c r="Q10" s="25"/>
-      <c r="R10" s="55" t="e">
+      <c r="R10" s="55">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
       <c r="S10" s="59" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T10" s="59" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="U10" s="59" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="V10" s="59" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="W10" s="59" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="X10" s="59" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
@@ -4032,29 +4235,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T11" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="U11" s="59" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="V11" s="59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="W11" s="59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="X11" s="59" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
@@ -4079,29 +4282,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="59" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T12" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="U12" s="59" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="V12" s="59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="W12" s="59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="X12" s="59" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
     <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
@@ -4126,29 +4329,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="59" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="T13" s="59" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="U13" s="59" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="W13" s="59" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="X13" s="59" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
     <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
@@ -4173,29 +4376,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="59" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T14" s="59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="U14" s="59" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="V14" s="59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="W14" s="59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="X14" s="59" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B15" s="18">
         <f>SUM(B4:B14)</f>
@@ -4203,23 +4406,23 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.9000000000000001</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.8500000000000003</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="4"/>
@@ -4273,28 +4476,28 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>7.4000000000000012</v>
       </c>
       <c r="H16" s="23">
         <f t="shared" si="5"/>
@@ -4361,34 +4564,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
-    <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006ADDC452BAA29F4C8DFF23CBF94E7959" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bf45315bdcdcd4c2a95595ea8a6a1800">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c873a42-625d-47d5-b5bc-361386e8fb0a" xmlns:ns4="776e5072-cb78-42ca-8229-d27cfde3db6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9dfe88d7c1f4e6e35cf6f7d6a3388ef" ns3:_="" ns4:_="">
+    <xsd:import namespace="2c873a42-625d-47d5-b5bc-361386e8fb0a"/>
+    <xsd:import namespace="776e5072-cb78-42ca-8229-d27cfde3db6a"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4396,61 +4589,67 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2c873a42-625d-47d5-b5bc-361386e8fb0a" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="776e5072-cb78-42ca-8229-d27cfde3db6a" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_activity" ma:index="11" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4553,28 +4752,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <_activity xmlns="776e5072-cb78-42ca-8229-d27cfde3db6a" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD665665-C76B-4E3B-924E-A72EA63A884D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="2c873a42-625d-47d5-b5bc-361386e8fb0a"/>
+    <ds:schemaRef ds:uri="776e5072-cb78-42ca-8229-d27cfde3db6a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -4585,18 +4788,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="776e5072-cb78-42ca-8229-d27cfde3db6a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c873a42-625d-47d5-b5bc-361386e8fb0a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Submission sprint 2 version.
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btmic\Desktop\GitHub\lei-24-s2-1dh-g084\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1230744_isep_ipp_pt/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B341F13-7D6B-4140-BA12-7ACFB5531A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8A4B95-9B91-4CE5-A7B8-2AA0C7DAE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -479,7 +479,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,8 +531,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +558,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -1001,7 +1020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1170,6 +1189,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1438,9 +1463,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1478,7 +1503,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1584,7 +1609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1726,7 +1751,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1737,37 +1762,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="5.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.9140625" customWidth="1"/>
+    <col min="4" max="19" width="7.875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="21">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20">
       <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1778,35 +1803,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" ht="16.149999999999999" thickBot="1"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="67"/>
-    </row>
-    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
+    </row>
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -1873,15 +1898,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B10" s="62" t="s">
+    <row r="10" spans="1:20">
+      <c r="B10" s="64" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="37">
         <v>1230399</v>
       </c>
       <c r="D10" s="36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="38">
         <v>4</v>
@@ -1907,11 +1932,11 @@
       <c r="R10" s="37"/>
       <c r="S10" s="50">
         <f>AVERAGE(D10:R10)</f>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B11" s="63"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="B11" s="65"/>
       <c r="C11" s="8">
         <v>1230741</v>
       </c>
@@ -1945,8 +1970,8 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B12" s="63"/>
+    <row r="12" spans="1:20">
+      <c r="B12" s="65"/>
       <c r="C12" s="8">
         <v>1231235</v>
       </c>
@@ -1980,8 +2005,8 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B13" s="63"/>
+    <row r="13" spans="1:20">
+      <c r="B13" s="65"/>
       <c r="C13" s="8">
         <v>1230744</v>
       </c>
@@ -2015,8 +2040,8 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B14" s="63"/>
+    <row r="14" spans="1:20">
+      <c r="B14" s="65"/>
       <c r="C14" s="8">
         <v>1191647</v>
       </c>
@@ -2050,8 +2075,8 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="63"/>
+    <row r="15" spans="1:20" ht="16.149999999999999" thickBot="1">
+      <c r="B15" s="65"/>
       <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
@@ -2075,8 +2100,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="63"/>
+    <row r="16" spans="1:20" ht="16.149999999999999" thickBot="1">
+      <c r="B16" s="65"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2100,8 +2125,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B17" s="65"/>
       <c r="C17" s="8" t="s">
         <v>8</v>
       </c>
@@ -2125,8 +2150,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="63"/>
+    <row r="18" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B18" s="65"/>
       <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
@@ -2150,8 +2175,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="63"/>
+    <row r="19" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B19" s="65"/>
       <c r="C19" s="8" t="s">
         <v>8</v>
       </c>
@@ -2175,8 +2200,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="63"/>
+    <row r="20" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B20" s="65"/>
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
@@ -2200,8 +2225,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="63"/>
+    <row r="21" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B21" s="65"/>
       <c r="C21" s="8" t="s">
         <v>8</v>
       </c>
@@ -2225,8 +2250,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="63"/>
+    <row r="22" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B22" s="65"/>
       <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
@@ -2250,8 +2275,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="63"/>
+    <row r="23" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B23" s="65"/>
       <c r="C23" s="8" t="s">
         <v>8</v>
       </c>
@@ -2275,8 +2300,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="64"/>
+    <row r="24" spans="1:19" ht="16.149999999999999" thickBot="1">
+      <c r="B24" s="66"/>
       <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
@@ -2300,14 +2325,14 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:19" ht="16.149999999999999" thickBot="1">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
@@ -2367,27 +2392,27 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19">
       <c r="A27" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19">
       <c r="A29" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2395,7 +2420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2403,7 +2428,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2411,7 +2436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2419,7 +2444,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2427,7 +2452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2455,35 +2480,35 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="62" t="s">
+    <row r="2" spans="1:10" ht="16.149999999999999" thickBot="1"/>
+    <row r="3" spans="1:10">
+      <c r="A3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="70" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="11">
@@ -2505,11 +2530,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="63"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="69"/>
+    <row r="4" spans="1:10" ht="31.15">
+      <c r="A4" s="65"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="14" t="s">
         <v>24</v>
       </c>
@@ -2529,11 +2554,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="63"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="69"/>
+    <row r="5" spans="1:10" ht="47.45" thickBot="1">
+      <c r="A5" s="65"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="22" t="s">
         <v>30</v>
       </c>
@@ -2553,7 +2578,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="46.9">
       <c r="A6" s="14">
         <v>1</v>
       </c>
@@ -2585,15 +2610,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="46.9">
       <c r="A7" s="14">
         <v>2</v>
       </c>
       <c r="B7" s="29">
-        <v>1230399</v>
+        <v>1230744</v>
       </c>
       <c r="C7" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="60">
         <v>4</v>
@@ -2617,15 +2642,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="46.9">
       <c r="A8" s="14">
         <v>3</v>
       </c>
       <c r="B8" s="29">
-        <v>1230399</v>
+        <v>1230744</v>
       </c>
       <c r="C8" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="60">
         <v>3</v>
@@ -2649,18 +2674,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="46.9">
       <c r="A9" s="14">
         <v>4</v>
       </c>
       <c r="B9" s="29">
-        <v>1230744</v>
+        <v>1230399</v>
       </c>
       <c r="C9" s="29">
         <v>3</v>
       </c>
       <c r="D9" s="60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>30</v>
@@ -2681,7 +2706,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="46.9">
       <c r="A10" s="14">
         <v>5</v>
       </c>
@@ -2713,7 +2738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="46.9">
       <c r="A11" s="14">
         <v>6</v>
       </c>
@@ -2745,7 +2770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="46.9">
       <c r="A12" s="14">
         <v>7</v>
       </c>
@@ -2777,7 +2802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="46.9">
       <c r="A13" s="14">
         <v>8</v>
       </c>
@@ -2809,11 +2834,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="60"/>
+    <row r="14" spans="1:10" ht="46.9">
+      <c r="A14" s="14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1230399</v>
+      </c>
+      <c r="C14" s="29">
+        <v>3</v>
+      </c>
+      <c r="D14" s="60">
+        <v>3</v>
+      </c>
       <c r="E14" s="14" t="s">
         <v>30</v>
       </c>
@@ -2833,11 +2866,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="60"/>
+    <row r="15" spans="1:10" ht="46.9">
+      <c r="A15" s="14">
+        <v>10</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1191647</v>
+      </c>
+      <c r="C15" s="29">
+        <v>3</v>
+      </c>
+      <c r="D15" s="60">
+        <v>3</v>
+      </c>
       <c r="E15" s="14" t="s">
         <v>30</v>
       </c>
@@ -2857,11 +2898,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="60"/>
+    <row r="16" spans="1:10" ht="46.9">
+      <c r="A16" s="14">
+        <v>11</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1230744</v>
+      </c>
+      <c r="C16" s="29">
+        <v>3</v>
+      </c>
+      <c r="D16" s="60">
+        <v>3</v>
+      </c>
       <c r="E16" s="14" t="s">
         <v>30</v>
       </c>
@@ -2881,11 +2930,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="60"/>
+    <row r="17" spans="1:10" ht="46.9">
+      <c r="A17" s="14">
+        <v>12</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1230741</v>
+      </c>
+      <c r="C17" s="29">
+        <v>3</v>
+      </c>
+      <c r="D17" s="60">
+        <v>3</v>
+      </c>
       <c r="E17" s="14" t="s">
         <v>30</v>
       </c>
@@ -2905,11 +2962,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="60"/>
+    <row r="18" spans="1:10" ht="46.9">
+      <c r="A18" s="14">
+        <v>13</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1191647</v>
+      </c>
+      <c r="C18" s="29">
+        <v>3</v>
+      </c>
+      <c r="D18" s="60">
+        <v>3</v>
+      </c>
       <c r="E18" s="14" t="s">
         <v>30</v>
       </c>
@@ -2929,12 +2994,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="14" t="s">
+    <row r="19" spans="1:10" ht="46.9">
+      <c r="A19" s="14">
+        <v>14</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1231235</v>
+      </c>
+      <c r="C19" s="29">
+        <v>3</v>
+      </c>
+      <c r="D19" s="60">
+        <v>4</v>
+      </c>
+      <c r="E19" s="63" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -2943,7 +3016,7 @@
       <c r="G19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="62" t="s">
         <v>33</v>
       </c>
       <c r="I19" s="7" t="s">
@@ -2953,7 +3026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="46.9">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -2977,7 +3050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="46.9">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -3001,7 +3074,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="46.9">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -3025,7 +3098,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="46.9">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -3049,7 +3122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="46.9">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -3073,7 +3146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" ht="47.45" thickBot="1">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -3110,10 +3183,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C25" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$E$40:$J$40</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C17" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C19" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$E$3:$J$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3139,27 +3212,27 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.9140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.58203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.9140625" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="24" t="s">
         <v>37</v>
       </c>
@@ -3178,8 +3251,8 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:26" ht="49" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="16.149999999999999" thickBot="1"/>
+    <row r="3" spans="1:26" ht="49.15">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3280,7 +3353,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="62.45">
       <c r="A4" s="14" t="s">
         <v>41</v>
       </c>
@@ -3337,7 +3410,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="124.9">
       <c r="A5" s="14" t="s">
         <v>48</v>
       </c>
@@ -3357,7 +3430,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -3371,7 +3444,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>49</v>
@@ -3394,7 +3467,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="78">
       <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
@@ -3405,7 +3478,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="25">
         <v>3</v>
@@ -3414,7 +3487,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -3451,18 +3524,28 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="93" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="93.6">
       <c r="A7" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="25">
+        <v>3</v>
+      </c>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="25">
+        <v>3</v>
+      </c>
+      <c r="F7" s="25">
+        <v>4</v>
+      </c>
+      <c r="G7" s="25">
+        <v>3</v>
+      </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
@@ -3473,9 +3556,9 @@
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="27" t="e">
+      <c r="R7" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>3.2</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>62</v>
@@ -3498,7 +3581,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26">
       <c r="A8" s="14" t="s">
         <v>67</v>
       </c>
@@ -3508,23 +3591,23 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
-        <v>2.7</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="1"/>
-        <v>2.7</v>
+        <v>3.8000000000000003</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>2.7</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>3.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="H8" s="7">
         <f t="shared" si="1"/>
@@ -3576,30 +3659,30 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="16.149999999999999" thickBot="1">
       <c r="A9" s="22" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
-        <v>10.8</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
-        <v>10.8</v>
+        <v>15.2</v>
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>10.8</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
-        <v>13.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="2"/>
-        <v>12.8</v>
+        <v>12.4</v>
       </c>
       <c r="H9" s="23">
         <f t="shared" si="2"/>
@@ -3651,7 +3734,7 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -3670,26 +3753,26 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.9140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.58203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.58203125" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.4140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.9140625" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21">
       <c r="A1" s="24" t="s">
         <v>69</v>
       </c>
@@ -3708,7 +3791,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="49" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="49.9">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3809,7 +3892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1">
       <c r="A4" s="14" t="s">
         <v>70</v>
       </c>
@@ -3866,7 +3949,7 @@
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>77</v>
       </c>
@@ -3923,7 +4006,7 @@
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="46.9">
       <c r="A6" s="14" t="s">
         <v>84</v>
       </c>
@@ -3980,7 +4063,7 @@
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="46.9">
       <c r="A7" s="14" t="s">
         <v>91</v>
       </c>
@@ -4037,7 +4120,7 @@
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="62.45">
       <c r="A8" s="14" t="s">
         <v>97</v>
       </c>
@@ -4094,7 +4177,7 @@
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="62.45">
       <c r="A9" s="14" t="s">
         <v>103</v>
       </c>
@@ -4147,7 +4230,7 @@
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="93.6">
       <c r="A10" s="14" t="s">
         <v>108</v>
       </c>
@@ -4204,7 +4287,7 @@
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="31.15">
       <c r="A11" s="14" t="s">
         <v>114</v>
       </c>
@@ -4251,18 +4334,28 @@
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="31.15">
       <c r="A12" s="14" t="s">
         <v>120</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="C12" s="25">
+        <v>3</v>
+      </c>
+      <c r="D12" s="25">
+        <v>4</v>
+      </c>
+      <c r="E12" s="25">
+        <v>4</v>
+      </c>
+      <c r="F12" s="25">
+        <v>4</v>
+      </c>
+      <c r="G12" s="25">
+        <v>3</v>
+      </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
@@ -4273,9 +4366,9 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
       <c r="Q12" s="25"/>
-      <c r="R12" s="55" t="e">
+      <c r="R12" s="55">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3.6</v>
       </c>
       <c r="S12" s="59" t="s">
         <v>104</v>
@@ -4298,18 +4391,28 @@
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="46.9">
       <c r="A13" s="14" t="s">
         <v>121</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="C13" s="25">
+        <v>4</v>
+      </c>
+      <c r="D13" s="25">
+        <v>4</v>
+      </c>
+      <c r="E13" s="25">
+        <v>4</v>
+      </c>
+      <c r="F13" s="25">
+        <v>4</v>
+      </c>
+      <c r="G13" s="25">
+        <v>3</v>
+      </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
@@ -4320,9 +4423,9 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
       <c r="Q13" s="25"/>
-      <c r="R13" s="55" t="e">
+      <c r="R13" s="55">
         <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>#DIV/0!</v>
+        <v>3.8</v>
       </c>
       <c r="S13" s="59" t="s">
         <v>122</v>
@@ -4345,18 +4448,28 @@
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="31.15">
       <c r="A14" s="14" t="s">
         <v>128</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="C14" s="25">
+        <v>3</v>
+      </c>
+      <c r="D14" s="25">
+        <v>4</v>
+      </c>
+      <c r="E14" s="25">
+        <v>4</v>
+      </c>
+      <c r="F14" s="25">
+        <v>4</v>
+      </c>
+      <c r="G14" s="25">
+        <v>3</v>
+      </c>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
@@ -4367,9 +4480,9 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
-      <c r="R14" s="55" t="e">
+      <c r="R14" s="55">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>3.6</v>
       </c>
       <c r="S14" s="59" t="s">
         <v>104</v>
@@ -4392,7 +4505,7 @@
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26">
       <c r="A15" s="14" t="s">
         <v>67</v>
       </c>
@@ -4402,23 +4515,23 @@
       </c>
       <c r="C15" s="7">
         <f>SUMPRODUCT(C4:C14,$B$4:$B$14)</f>
-        <v>2</v>
+        <v>3.1499999999999995</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" ref="D15:Q15" si="4">SUMPRODUCT(D4:D14,$B$4:$B$14)</f>
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>1.9000000000000001</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>2.0499999999999998</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
-        <v>1.8500000000000003</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="H15" s="7">
         <f t="shared" si="4"/>
@@ -4470,30 +4583,30 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26">
       <c r="A16" s="22" t="s">
         <v>68</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
         <f>C15/5*20</f>
-        <v>8</v>
+        <v>12.599999999999998</v>
       </c>
       <c r="D16" s="23">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>8</v>
+        <v>13.599999999999998</v>
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>7.6</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
-        <v>8.1999999999999993</v>
+        <v>13.799999999999999</v>
       </c>
       <c r="G16" s="23">
         <f t="shared" si="5"/>
-        <v>7.4000000000000012</v>
+        <v>11.600000000000001</v>
       </c>
       <c r="H16" s="23">
         <f t="shared" si="5"/>
@@ -4545,7 +4658,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -4766,45 +4879,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD665665-C76B-4E3B-924E-A72EA63A884D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c873a42-625d-47d5-b5bc-361386e8fb0a"/>
-    <ds:schemaRef ds:uri="776e5072-cb78-42ca-8229-d27cfde3db6a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD665665-C76B-4E3B-924E-A72EA63A884D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="776e5072-cb78-42ca-8229-d27cfde3db6a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2c873a42-625d-47d5-b5bc-361386e8fb0a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}"/>
 </file>
</xml_diff>